<commit_message>
error fix, change log, other miscellaneous edits
Created a changelog with details of updates. It will list all changes made to the new version and on what dates those changes were made.
</commit_message>
<xml_diff>
--- a/CodeBook_7_27_2020.xlsx
+++ b/CodeBook_7_27_2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rachel/Desktop/Raifman project/Code book and primary documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF856A38-CF91-AF49-B569-A5BDE5EECB16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89EDFDE-95E8-8F49-A947-5DD6AFDA7E70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="2960" windowWidth="28080" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="525">
   <si>
     <t>people/year</t>
   </si>
@@ -1515,12 +1515,6 @@
     <t>0: policy not implemented; valid date range: 4/20/2020, 6/22/2020</t>
   </si>
   <si>
-    <t>0: policy not implemented; valid date range: 6/26/2020, 7/14/2020</t>
-  </si>
-  <si>
-    <t>0: policy not implemented; valid date range: 6/26/2020, 7/16/2020</t>
-  </si>
-  <si>
     <t>0: policy not implemented; valid date range: 6/26/2020, 7/13/2020</t>
   </si>
   <si>
@@ -1653,10 +1647,13 @@
     <t>The date states allowed audio only telehealth statewide. If a state previously allowed audio only telehealth, it will be marked as 1/0/1900</t>
   </si>
   <si>
-    <t>0: No change in status/policy not implemented;  invalid date range:</t>
-  </si>
-  <si>
     <t>Whether a state suspended their non-payment lock-out policy for CHIP during the pandemic. If a state did not have an existing lock-out policy, they will be marked as 0.</t>
+  </si>
+  <si>
+    <t>0: No change in status/policy not implemented; valid date range: 5/1/2020, 7/28/2020</t>
+  </si>
+  <si>
+    <t>0: policy not implemented; valid date range: 6/26/2020, 7/28/2020</t>
   </si>
 </sst>
 </file>
@@ -2163,8 +2160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C43" zoomScale="93" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="93" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -2367,7 +2364,7 @@
         <v>138</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>32</v>
@@ -2810,7 +2807,7 @@
       <c r="H24" s="6"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>234</v>
       </c>
@@ -2818,7 +2815,7 @@
         <v>121</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>25</v>
@@ -2895,7 +2892,7 @@
         <v>118</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>25</v>
@@ -2945,7 +2942,7 @@
         <v>116</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>25</v>
@@ -2995,7 +2992,7 @@
         <v>114</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>25</v>
@@ -3020,7 +3017,7 @@
         <v>113</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>25</v>
@@ -3045,7 +3042,7 @@
         <v>112</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D34" s="13" t="s">
         <v>25</v>
@@ -3070,7 +3067,7 @@
         <v>111</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D35" s="13" t="s">
         <v>25</v>
@@ -3095,7 +3092,7 @@
         <v>110</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D36" s="13" t="s">
         <v>25</v>
@@ -3122,7 +3119,7 @@
         <v>109</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>24</v>
@@ -3134,7 +3131,7 @@
         <v>4</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>478</v>
+        <v>524</v>
       </c>
       <c r="H37" s="18"/>
       <c r="I37" s="19" t="s">
@@ -3149,7 +3146,7 @@
         <v>108</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>24</v>
@@ -3161,7 +3158,7 @@
         <v>4</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>479</v>
+        <v>524</v>
       </c>
       <c r="H38" s="18"/>
       <c r="I38" s="19" t="s">
@@ -3176,7 +3173,7 @@
         <v>107</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>24</v>
@@ -3188,7 +3185,7 @@
         <v>4</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="H39" s="18"/>
       <c r="I39" s="20" t="s">
@@ -3203,7 +3200,7 @@
         <v>106</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>24</v>
@@ -3215,7 +3212,7 @@
         <v>4</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="H40" s="18"/>
       <c r="I40" s="20" t="s">
@@ -3230,7 +3227,7 @@
         <v>300</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>24</v>
@@ -3242,7 +3239,7 @@
         <v>4</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="H41" s="18"/>
       <c r="I41" s="20"/>
@@ -3267,7 +3264,7 @@
         <v>4</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="H42" s="18"/>
       <c r="I42" s="19" t="s">
@@ -3294,7 +3291,7 @@
         <v>4</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="H43" s="18"/>
       <c r="I43" s="19"/>
@@ -3319,7 +3316,7 @@
         <v>4</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H44" s="18"/>
       <c r="I44" s="19"/>
@@ -3344,7 +3341,7 @@
         <v>4</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="H45" s="6"/>
       <c r="I45" s="19"/>
@@ -3369,7 +3366,7 @@
         <v>4</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="H46" s="6"/>
       <c r="I46" s="19"/>
@@ -3394,7 +3391,7 @@
         <v>4</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="H47" s="6"/>
       <c r="I47" s="19"/>
@@ -3419,7 +3416,7 @@
         <v>4</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="H48" s="6"/>
       <c r="I48" s="19" t="s">
@@ -3446,7 +3443,7 @@
         <v>4</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="H49" s="6"/>
       <c r="I49" s="19"/>
@@ -3471,7 +3468,7 @@
         <v>4</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="H50" s="6"/>
       <c r="I50" s="19"/>
@@ -3496,7 +3493,7 @@
         <v>4</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="H51" s="6"/>
       <c r="I51" s="19" t="s">
@@ -3523,7 +3520,7 @@
         <v>4</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="H52" s="6"/>
       <c r="I52" s="21" t="s">
@@ -3550,7 +3547,7 @@
         <v>4</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="H53" s="6"/>
       <c r="I53" s="19" t="s">
@@ -3606,7 +3603,7 @@
         <v>4</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="H55" s="6"/>
       <c r="I55" s="19" t="s">
@@ -3633,7 +3630,7 @@
         <v>4</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="H56" s="6"/>
       <c r="I56" s="19"/>
@@ -3675,7 +3672,7 @@
         <v>90</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>17</v>
@@ -3687,7 +3684,7 @@
         <v>4</v>
       </c>
       <c r="G58" s="8" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="H58" s="6"/>
       <c r="I58" s="19"/>
@@ -3712,7 +3709,7 @@
         <v>4</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="H59" s="6"/>
       <c r="I59" s="19"/>
@@ -3754,7 +3751,7 @@
         <v>87</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>17</v>
@@ -4470,7 +4467,7 @@
         <v>4</v>
       </c>
       <c r="G87" s="8" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="H87" s="6"/>
       <c r="I87" s="19"/>
@@ -4495,7 +4492,7 @@
         <v>4</v>
       </c>
       <c r="G88" s="8" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H88" s="6"/>
       <c r="I88" s="19"/>
@@ -4636,7 +4633,7 @@
         <v>4</v>
       </c>
       <c r="G93" s="8" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H93" s="6"/>
       <c r="I93" s="19"/>
@@ -4649,7 +4646,7 @@
         <v>361</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D94" s="6" t="s">
         <v>17</v>
@@ -4661,7 +4658,7 @@
         <v>4</v>
       </c>
       <c r="G94" s="8" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="H94" s="6"/>
       <c r="I94" s="19"/>
@@ -4713,7 +4710,7 @@
         <v>4</v>
       </c>
       <c r="G96" s="8" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="H96" s="6"/>
       <c r="I96" s="19" t="s">
@@ -5013,7 +5010,7 @@
         <v>4</v>
       </c>
       <c r="G107" s="8" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="H107" s="6" t="s">
         <v>294</v>
@@ -5040,7 +5037,7 @@
         <v>4</v>
       </c>
       <c r="G108" s="8" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="H108" s="6"/>
       <c r="I108" s="19"/>
@@ -5065,7 +5062,7 @@
         <v>4</v>
       </c>
       <c r="G109" s="8" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="H109" s="6"/>
       <c r="I109" s="19"/>
@@ -5090,7 +5087,7 @@
         <v>4</v>
       </c>
       <c r="G110" s="8" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="H110" s="6"/>
       <c r="I110" s="19"/>
@@ -5115,7 +5112,7 @@
         <v>4</v>
       </c>
       <c r="G111" s="8" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H111" s="6"/>
       <c r="I111" s="19"/>
@@ -5140,7 +5137,7 @@
         <v>4</v>
       </c>
       <c r="G112" s="8" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="H112" s="6"/>
       <c r="I112" s="19"/>

</xml_diff>